<commit_message>
Add estimator versioning info
</commit_message>
<xml_diff>
--- a/_assets/documents/cloud-gov-cost-estimator.xlsx
+++ b/_assets/documents/cloud-gov-cost-estimator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterdburkholder/Projects/cloud-gov/cg-site/_assets/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CC62A2-CA76-6647-8B57-70FB1B3E5486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F2CCC5-A8FF-6241-AE0E-4F14A78F5FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="500" windowWidth="47840" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="500" windowWidth="47840" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="190">
   <si>
     <t>Estimated Price</t>
   </si>
@@ -624,19 +624,42 @@
 - For services that AWS bills hourly, we bill based on the total instances operating at the end of the month. 
 - To create an estimate, average your usage over the month.</t>
   </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Add versions</t>
+  </si>
+  <si>
+    <t>Fix metered calcs</t>
+  </si>
+  <si>
+    <t>Add unit/credit info</t>
+  </si>
+  <si>
+    <t>Initial version</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="5">
+  <numFmts count="7">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0000"/>
     <numFmt numFmtId="167" formatCode="0\ &quot;Gb&quot;"/>
     <numFmt numFmtId="168" formatCode="0\ &quot;Hrs&quot;"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -696,8 +719,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -750,6 +786,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
         <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1395,10 +1437,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1633,10 +1676,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1669,22 +1708,30 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="69">
     <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="170" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -1771,281 +1818,18 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF284E3F"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFFFFFF"/>
-        </top>
+      <border outline="0">
         <bottom style="thin">
-          <color rgb="FF284E3F"/>
+          <color rgb="FF4A535C"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="0\ &quot;Gb&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFFFFFF"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF284E3F"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFFFFFF"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF284E3F"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFFFFFF"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF284E3F"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFFFFFF"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF284E3F"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF284E3F"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFFFFFF"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF284E3F"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2077,6 +1861,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2348,6 +2133,63 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0\ &quot;Hrs&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF284E3F"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="167" formatCode="0\ &quot;Gb&quot;"/>
       <fill>
         <patternFill patternType="solid">
@@ -2480,6 +2322,36 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="1"/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0\ &quot;Gb&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFFF0000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFFF0000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFFF0000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2495,11 +2367,165 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0\ &quot;Hrs&quot;"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0000"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF284E3F"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2988,54 +3014,54 @@
   </dxfs>
   <tableStyles count="10">
     <tableStyle name="Worksheet-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="69"/>
-      <tableStyleElement type="firstRowStripe" dxfId="68"/>
-      <tableStyleElement type="secondRowStripe" dxfId="67"/>
+      <tableStyleElement type="headerRow" dxfId="68"/>
+      <tableStyleElement type="firstRowStripe" dxfId="67"/>
+      <tableStyleElement type="secondRowStripe" dxfId="66"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="66"/>
-      <tableStyleElement type="firstRowStripe" dxfId="65"/>
-      <tableStyleElement type="secondRowStripe" dxfId="64"/>
+      <tableStyleElement type="headerRow" dxfId="65"/>
+      <tableStyleElement type="firstRowStripe" dxfId="64"/>
+      <tableStyleElement type="secondRowStripe" dxfId="63"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="63"/>
-      <tableStyleElement type="firstRowStripe" dxfId="62"/>
-      <tableStyleElement type="secondRowStripe" dxfId="61"/>
+      <tableStyleElement type="headerRow" dxfId="62"/>
+      <tableStyleElement type="firstRowStripe" dxfId="61"/>
+      <tableStyleElement type="secondRowStripe" dxfId="60"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="headerRow" dxfId="60"/>
-      <tableStyleElement type="firstRowStripe" dxfId="59"/>
-      <tableStyleElement type="secondRowStripe" dxfId="58"/>
+      <tableStyleElement type="headerRow" dxfId="59"/>
+      <tableStyleElement type="firstRowStripe" dxfId="58"/>
+      <tableStyleElement type="secondRowStripe" dxfId="57"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 5" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
-      <tableStyleElement type="headerRow" dxfId="57"/>
-      <tableStyleElement type="firstRowStripe" dxfId="56"/>
-      <tableStyleElement type="secondRowStripe" dxfId="55"/>
+      <tableStyleElement type="headerRow" dxfId="56"/>
+      <tableStyleElement type="firstRowStripe" dxfId="55"/>
+      <tableStyleElement type="secondRowStripe" dxfId="54"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 6" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
-      <tableStyleElement type="headerRow" dxfId="54"/>
-      <tableStyleElement type="firstRowStripe" dxfId="53"/>
-      <tableStyleElement type="secondRowStripe" dxfId="52"/>
+      <tableStyleElement type="headerRow" dxfId="53"/>
+      <tableStyleElement type="firstRowStripe" dxfId="52"/>
+      <tableStyleElement type="secondRowStripe" dxfId="51"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 7" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
-      <tableStyleElement type="headerRow" dxfId="51"/>
-      <tableStyleElement type="firstRowStripe" dxfId="50"/>
-      <tableStyleElement type="secondRowStripe" dxfId="49"/>
+      <tableStyleElement type="headerRow" dxfId="50"/>
+      <tableStyleElement type="firstRowStripe" dxfId="49"/>
+      <tableStyleElement type="secondRowStripe" dxfId="48"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 8" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF07000000}">
-      <tableStyleElement type="headerRow" dxfId="48"/>
-      <tableStyleElement type="firstRowStripe" dxfId="47"/>
-      <tableStyleElement type="secondRowStripe" dxfId="46"/>
+      <tableStyleElement type="headerRow" dxfId="47"/>
+      <tableStyleElement type="firstRowStripe" dxfId="46"/>
+      <tableStyleElement type="secondRowStripe" dxfId="45"/>
     </tableStyle>
     <tableStyle name="Cloud.gov Tiers-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF08000000}">
-      <tableStyleElement type="headerRow" dxfId="45"/>
-      <tableStyleElement type="firstRowStripe" dxfId="44"/>
-      <tableStyleElement type="secondRowStripe" dxfId="43"/>
+      <tableStyleElement type="headerRow" dxfId="44"/>
+      <tableStyleElement type="firstRowStripe" dxfId="43"/>
+      <tableStyleElement type="secondRowStripe" dxfId="42"/>
     </tableStyle>
     <tableStyle name="Cloud.gov Tiers-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF09000000}">
-      <tableStyleElement type="headerRow" dxfId="42"/>
-      <tableStyleElement type="firstRowStripe" dxfId="41"/>
-      <tableStyleElement type="secondRowStripe" dxfId="40"/>
+      <tableStyleElement type="headerRow" dxfId="41"/>
+      <tableStyleElement type="firstRowStripe" dxfId="40"/>
+      <tableStyleElement type="secondRowStripe" dxfId="39"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -3052,20 +3078,20 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A4:F5">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Credits" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tier Name" dataDxfId="38">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Credits" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tier Name" dataDxfId="37">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.Tier, VLOOKUP(MIN(IF('Cloud.gov Tiers'!$B$11:$B$28&gt;=A5, 'Cloud.gov Tiers'!$B$11:$B$28)), 'Cloud.gov Tiers'!$B$11:$E$28, 4, FALSE), VLOOKUP(_xlpm.Tier, 'Cloud.gov Tiers'!$E$10:$F$28, 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Credits Remaining_x000a_in Tier" dataDxfId="37">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Credits Remaining_x000a_in Tier" dataDxfId="36">
       <calculatedColumnFormula>VLOOKUP(Table_1[[#This Row],[Tier Name]], 'Cloud.gov Tiers'!A11:B27, 2,FALSE)-Table_1[[#This Row],[Credits]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Yearly_x000a_Platform Total" dataDxfId="36">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Yearly_x000a_Platform Total" dataDxfId="35">
       <calculatedColumnFormula>IF(B5="Custom", ROUNDUP(A5/1000,0)*'Cloud.gov Tiers'!$H$28, VLOOKUP(B5, 'Cloud.gov Tiers'!$F$11:$H$27, 3, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Support Total" dataDxfId="35">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Support Total" dataDxfId="34">
       <calculatedColumnFormula>C15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name=" YearlyTotal Cost" dataDxfId="34">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name=" YearlyTotal Cost" dataDxfId="33">
       <calculatedColumnFormula>D5+E5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3074,6 +3100,16 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table_9" displayName="Table_9" ref="A2:B6">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Variable"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="Cloud.gov Tiers-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table_10" displayName="Table_10" ref="A10:H28">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Tier"/>
@@ -3093,7 +3129,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A9:C10">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Resource"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Quantity" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Quantity" dataDxfId="32"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Credits"/>
   </tableColumns>
   <tableStyleInfo name="Worksheet-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -3103,13 +3139,13 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="E9:K10">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Offering" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Description" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Dimension" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="GB per credit" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Quantity (GB)" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Credits" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Offering" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Description" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Dimension" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="GB per credit" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Quantity (GB)" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Credits" dataDxfId="25">
       <calculatedColumnFormula>ROUNDUP(Table_3[[#This Row],[Quantity (GB)]]/Table_3[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3123,12 +3159,12 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Offering"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Units"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Dimension" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{CDA60C5E-AE6A-324F-8F61-A71F1A0A8966}" name="GB per credit" dataDxfId="29">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Dimension" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{CDA60C5E-AE6A-324F-8F61-A71F1A0A8966}" name="GB per credit" dataDxfId="23">
       <calculatedColumnFormula>'AWS Service Prices'!K5*'AWS Service Prices'!M5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Quantity (GB)" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Credits" dataDxfId="30">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Quantity (GB)" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Credits" dataDxfId="21">
       <calculatedColumnFormula>ROUNDUP(Table_4[[#This Row],[Quantity (GB)]]/Table_4[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3140,7 +3176,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="A14:C15">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Rate/Hour"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Hours" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Hours" dataDxfId="20"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Total"/>
   </tableColumns>
   <tableStyleInfo name="Worksheet-style 5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -3150,15 +3186,15 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_6" displayName="Table_6" ref="M14:S15" dataDxfId="19">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Offering" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Description" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Units" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Dimension" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{807927EE-801B-8148-9BA1-5FE9186170F2}" name="GB per credit" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Offering" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Description" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Units" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Dimension" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{807927EE-801B-8148-9BA1-5FE9186170F2}" name="GB per credit" dataDxfId="14">
       <calculatedColumnFormula>'AWS Service Prices'!K4*'AWS Service Prices'!M4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Quantity (GB)" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Credits" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Quantity (GB)" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Credits" dataDxfId="12">
       <calculatedColumnFormula>ROUNDUP(Table_6[[#This Row],[Quantity (GB)]]/Table_6[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3183,11 +3219,11 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Units"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Dimension"/>
-    <tableColumn id="3" xr3:uid="{A30E673E-5221-9442-BA33-5D5CC8E273B5}" name="Units/Credit" dataDxfId="31">
+    <tableColumn id="3" xr3:uid="{A30E673E-5221-9442-BA33-5D5CC8E273B5}" name="Units/Credit" dataDxfId="11">
       <calculatedColumnFormula>'AWS Service Prices'!K6*'AWS Service Prices'!M6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Quantity"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Credits" dataDxfId="18">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Credits" dataDxfId="10">
       <calculatedColumnFormula>ROUNDUP(Table_8[[#This Row],[Quantity]]/Table_8[[#This Row],[Units/Credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3196,12 +3232,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table_9" displayName="Table_9" ref="A2:B6">
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Variable"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Value"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}" name="Table12" displayName="Table12" ref="A39:C49" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="9">
+  <autoFilter ref="A39:C49" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6F594386-932F-3745-B570-1D36152A4BED}" name="Version" dataDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{98BA1600-A7B8-2742-AF88-1C465CCF83D5}" name="Date"/>
+    <tableColumn id="3" xr3:uid="{A3A06425-E98A-E042-A27B-C92165F08BCF}" name="Notes"/>
   </tableColumns>
-  <tableStyleInfo name="Cloud.gov Tiers-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="Cloud.gov Tiers-style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3410,14 +3448,14 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S42" sqref="S42"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="30.83203125" customWidth="1"/>
@@ -3440,14 +3478,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="98.25" customHeight="1" x14ac:dyDescent="1.05">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3703,7 +3741,7 @@
       <c r="J14" s="20">
         <v>2</v>
       </c>
-      <c r="K14" s="92">
+      <c r="K14" s="90">
         <f>I14*J14</f>
         <v>2</v>
       </c>
@@ -3758,7 +3796,7 @@
       <c r="J15" s="26">
         <v>0</v>
       </c>
-      <c r="K15" s="92">
+      <c r="K15" s="90">
         <f t="shared" ref="K15:K43" si="0">I15*J15</f>
         <v>0</v>
       </c>
@@ -3805,7 +3843,7 @@
       <c r="J16" s="26">
         <v>0</v>
       </c>
-      <c r="K16" s="92">
+      <c r="K16" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3832,7 +3870,7 @@
       <c r="J17" s="26">
         <v>1</v>
       </c>
-      <c r="K17" s="92">
+      <c r="K17" s="90">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -3866,7 +3904,7 @@
       <c r="J18" s="26">
         <v>0</v>
       </c>
-      <c r="K18" s="92">
+      <c r="K18" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3918,7 +3956,7 @@
       <c r="J19" s="26">
         <v>0</v>
       </c>
-      <c r="K19" s="92">
+      <c r="K19" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3972,7 +4010,7 @@
       <c r="J20" s="26">
         <v>0</v>
       </c>
-      <c r="K20" s="92">
+      <c r="K20" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4025,7 +4063,7 @@
       <c r="J21" s="26">
         <v>0</v>
       </c>
-      <c r="K21" s="92">
+      <c r="K21" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4078,7 +4116,7 @@
       <c r="J22" s="35">
         <v>0</v>
       </c>
-      <c r="K22" s="92">
+      <c r="K22" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4131,7 +4169,7 @@
       <c r="J23" s="26">
         <v>0</v>
       </c>
-      <c r="K23" s="92">
+      <c r="K23" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4177,7 +4215,7 @@
       <c r="J24" s="26">
         <v>0</v>
       </c>
-      <c r="K24" s="92">
+      <c r="K24" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4223,7 +4261,7 @@
       <c r="J25" s="26">
         <v>0</v>
       </c>
-      <c r="K25" s="92">
+      <c r="K25" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4272,7 +4310,7 @@
       <c r="J26" s="26">
         <v>0</v>
       </c>
-      <c r="K26" s="92">
+      <c r="K26" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4324,7 +4362,7 @@
       <c r="J27" s="26">
         <v>0</v>
       </c>
-      <c r="K27" s="92">
+      <c r="K27" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4377,7 +4415,7 @@
       <c r="J28" s="26">
         <v>0</v>
       </c>
-      <c r="K28" s="92">
+      <c r="K28" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4429,7 +4467,7 @@
       <c r="J29" s="26">
         <v>0</v>
       </c>
-      <c r="K29" s="92">
+      <c r="K29" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4451,11 +4489,11 @@
       <c r="R29" s="41">
         <v>0</v>
       </c>
-      <c r="S29" s="93">
+      <c r="S29" s="91">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T29" s="94"/>
+      <c r="T29" s="92"/>
     </row>
     <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="18" t="str">
@@ -4482,7 +4520,7 @@
       <c r="J30" s="43">
         <v>0</v>
       </c>
-      <c r="K30" s="92">
+      <c r="K30" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4514,7 +4552,7 @@
       <c r="J31" s="26">
         <v>0</v>
       </c>
-      <c r="K31" s="92">
+      <c r="K31" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4552,7 +4590,7 @@
       <c r="J32" s="26">
         <v>0</v>
       </c>
-      <c r="K32" s="92">
+      <c r="K32" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4603,7 +4641,7 @@
       <c r="J33" s="26">
         <v>0</v>
       </c>
-      <c r="K33" s="92">
+      <c r="K33" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4620,7 +4658,7 @@
       <c r="P33" s="48">
         <v>1</v>
       </c>
-      <c r="Q33" s="90">
+      <c r="Q33" s="88">
         <v>1</v>
       </c>
       <c r="R33" s="50">
@@ -4656,7 +4694,7 @@
       <c r="J34" s="26">
         <v>0</v>
       </c>
-      <c r="K34" s="92">
+      <c r="K34" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4672,7 +4710,7 @@
       <c r="P34" s="25">
         <v>3</v>
       </c>
-      <c r="Q34" s="90">
+      <c r="Q34" s="88">
         <v>2</v>
       </c>
       <c r="R34" s="38">
@@ -4708,7 +4746,7 @@
       <c r="J35" s="35">
         <v>0</v>
       </c>
-      <c r="K35" s="92">
+      <c r="K35" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4724,7 +4762,7 @@
       <c r="P35" s="48">
         <v>5</v>
       </c>
-      <c r="Q35" s="90">
+      <c r="Q35" s="88">
         <v>4</v>
       </c>
       <c r="R35" s="38">
@@ -4758,7 +4796,7 @@
       <c r="J36" s="26">
         <v>0</v>
       </c>
-      <c r="K36" s="92">
+      <c r="K36" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4774,7 +4812,7 @@
       <c r="P36" s="25">
         <v>3</v>
       </c>
-      <c r="Q36" s="90">
+      <c r="Q36" s="88">
         <v>5</v>
       </c>
       <c r="R36" s="38">
@@ -4804,7 +4842,7 @@
       <c r="J37" s="26">
         <v>0</v>
       </c>
-      <c r="K37" s="92">
+      <c r="K37" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4820,13 +4858,13 @@
       <c r="P37" s="40">
         <v>5</v>
       </c>
-      <c r="Q37" s="91">
+      <c r="Q37" s="89">
         <v>8</v>
       </c>
       <c r="R37" s="45">
         <v>0</v>
       </c>
-      <c r="S37" s="93">
+      <c r="S37" s="91">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4850,12 +4888,21 @@
       <c r="J38" s="26">
         <v>0</v>
       </c>
-      <c r="K38" s="92">
+      <c r="K38" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="104" t="s">
+        <v>183</v>
+      </c>
+      <c r="B39" s="105" t="s">
+        <v>184</v>
+      </c>
+      <c r="C39" s="106" t="s">
+        <v>185</v>
+      </c>
       <c r="E39" s="24" t="str">
         <v>AWS RDS</v>
       </c>
@@ -4874,7 +4921,7 @@
       <c r="J39" s="26">
         <v>0</v>
       </c>
-      <c r="K39" s="92">
+      <c r="K39" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4883,6 +4930,15 @@
       </c>
     </row>
     <row r="40" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="107">
+        <v>1</v>
+      </c>
+      <c r="B40" s="103">
+        <v>45748</v>
+      </c>
+      <c r="C40" s="102" t="s">
+        <v>189</v>
+      </c>
       <c r="E40" s="18" t="str">
         <v>AWS RDS</v>
       </c>
@@ -4901,7 +4957,7 @@
       <c r="J40" s="26">
         <v>0</v>
       </c>
-      <c r="K40" s="92">
+      <c r="K40" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4923,11 +4979,20 @@
       <c r="R40" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="S40" s="97" t="s">
+      <c r="S40" s="95" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="107">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B41" s="103">
+        <v>45749</v>
+      </c>
+      <c r="C41" s="102" t="s">
+        <v>186</v>
+      </c>
       <c r="E41" s="24" t="str">
         <v>AWS RDS</v>
       </c>
@@ -4946,7 +5011,7 @@
       <c r="J41" s="26">
         <v>0</v>
       </c>
-      <c r="K41" s="92">
+      <c r="K41" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4962,19 +5027,23 @@
       <c r="P41" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="Q41" s="90">
+      <c r="Q41" s="88">
         <f>'AWS Service Prices'!K6*'AWS Service Prices'!M6</f>
         <v>150000</v>
       </c>
-      <c r="R41" s="95">
+      <c r="R41" s="93">
         <v>10000</v>
       </c>
-      <c r="S41" s="99">
+      <c r="S41" s="97">
         <f>ROUNDUP(Table_8[[#This Row],[Quantity]]/Table_8[[#This Row],[Units/Credit]],0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="107"/>
+      <c r="C42" s="102" t="s">
+        <v>187</v>
+      </c>
       <c r="E42" s="18" t="str">
         <v>AWS RDS</v>
       </c>
@@ -4993,7 +5062,7 @@
       <c r="J42" s="26">
         <v>0</v>
       </c>
-      <c r="K42" s="92">
+      <c r="K42" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5009,19 +5078,23 @@
       <c r="P42" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="Q42" s="90">
+      <c r="Q42" s="88">
         <f>'AWS Service Prices'!K7*'AWS Service Prices'!M7</f>
         <v>120</v>
       </c>
-      <c r="R42" s="96">
+      <c r="R42" s="94">
         <v>2</v>
       </c>
-      <c r="S42" s="98">
+      <c r="S42" s="96">
         <f>ROUNDUP(Table_8[[#This Row],[Quantity]]/Table_8[[#This Row],[Units/Credit]],0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="107"/>
+      <c r="C43" s="102" t="s">
+        <v>188</v>
+      </c>
       <c r="E43" s="54" t="str">
         <v>AWS RDS</v>
       </c>
@@ -5040,73 +5113,80 @@
       <c r="J43" s="56">
         <v>0</v>
       </c>
-      <c r="K43" s="101">
+      <c r="K43" s="99">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q43" s="100"/>
+      <c r="Q43" s="98"/>
     </row>
     <row r="44" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="107"/>
       <c r="J44" s="4"/>
     </row>
     <row r="45" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="107"/>
       <c r="J45" s="4"/>
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="107"/>
       <c r="J46" s="4"/>
     </row>
     <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="107"/>
       <c r="J47" s="4"/>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="107"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="107"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="107"/>
       <c r="J50" s="4"/>
     </row>
-    <row r="51" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J52" s="4"/>
     </row>
-    <row r="53" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J54" s="4"/>
     </row>
-    <row r="55" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J58" s="4"/>
     </row>
-    <row r="59" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J59" s="4"/>
     </row>
-    <row r="60" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J60" s="4"/>
     </row>
-    <row r="61" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J61" s="4"/>
     </row>
-    <row r="62" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J62" s="4"/>
     </row>
-    <row r="63" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J63" s="4"/>
     </row>
-    <row r="64" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J64" s="4"/>
     </row>
     <row r="65" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6078,43 +6158,43 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="B10 J14:J43 B15">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R10">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R15">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R19:R29">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R33:R37">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R41:R42">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R19:R29">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R33:R37">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R15">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <tableParts count="8">
+  <tableParts count="9">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -6123,6 +6203,7 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7789,7 +7870,7 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="K3" sqref="K3:M3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add estimator versioning info (#2613)
</commit_message>
<xml_diff>
--- a/_assets/documents/cloud-gov-cost-estimator.xlsx
+++ b/_assets/documents/cloud-gov-cost-estimator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterdburkholder/Projects/cloud-gov/cg-site/_assets/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CC62A2-CA76-6647-8B57-70FB1B3E5486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F2CCC5-A8FF-6241-AE0E-4F14A78F5FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="500" windowWidth="47840" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="500" windowWidth="47840" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="190">
   <si>
     <t>Estimated Price</t>
   </si>
@@ -624,19 +624,42 @@
 - For services that AWS bills hourly, we bill based on the total instances operating at the end of the month. 
 - To create an estimate, average your usage over the month.</t>
   </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Add versions</t>
+  </si>
+  <si>
+    <t>Fix metered calcs</t>
+  </si>
+  <si>
+    <t>Add unit/credit info</t>
+  </si>
+  <si>
+    <t>Initial version</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="5">
+  <numFmts count="7">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0000"/>
     <numFmt numFmtId="167" formatCode="0\ &quot;Gb&quot;"/>
     <numFmt numFmtId="168" formatCode="0\ &quot;Hrs&quot;"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -696,8 +719,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -750,6 +786,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
         <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1395,10 +1437,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1633,10 +1676,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1669,22 +1708,30 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="69">
     <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="170" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -1771,281 +1818,18 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <u/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF284E3F"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFFFFFF"/>
-        </top>
+      <border outline="0">
         <bottom style="thin">
-          <color rgb="FF284E3F"/>
+          <color rgb="FF4A535C"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="0\ &quot;Gb&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFFFFFF"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF284E3F"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFFFFFF"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF284E3F"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFFFFFF"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF284E3F"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFFFFFF"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF284E3F"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF284E3F"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFFFFFF"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF284E3F"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2077,6 +1861,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2348,6 +2133,63 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0\ &quot;Hrs&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF284E3F"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="167" formatCode="0\ &quot;Gb&quot;"/>
       <fill>
         <patternFill patternType="solid">
@@ -2480,6 +2322,36 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="1"/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0\ &quot;Gb&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFFF0000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFFF0000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFFF0000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2495,11 +2367,165 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0\ &quot;Hrs&quot;"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0000"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF284E3F"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF284E3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2988,54 +3014,54 @@
   </dxfs>
   <tableStyles count="10">
     <tableStyle name="Worksheet-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="69"/>
-      <tableStyleElement type="firstRowStripe" dxfId="68"/>
-      <tableStyleElement type="secondRowStripe" dxfId="67"/>
+      <tableStyleElement type="headerRow" dxfId="68"/>
+      <tableStyleElement type="firstRowStripe" dxfId="67"/>
+      <tableStyleElement type="secondRowStripe" dxfId="66"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="66"/>
-      <tableStyleElement type="firstRowStripe" dxfId="65"/>
-      <tableStyleElement type="secondRowStripe" dxfId="64"/>
+      <tableStyleElement type="headerRow" dxfId="65"/>
+      <tableStyleElement type="firstRowStripe" dxfId="64"/>
+      <tableStyleElement type="secondRowStripe" dxfId="63"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="63"/>
-      <tableStyleElement type="firstRowStripe" dxfId="62"/>
-      <tableStyleElement type="secondRowStripe" dxfId="61"/>
+      <tableStyleElement type="headerRow" dxfId="62"/>
+      <tableStyleElement type="firstRowStripe" dxfId="61"/>
+      <tableStyleElement type="secondRowStripe" dxfId="60"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="headerRow" dxfId="60"/>
-      <tableStyleElement type="firstRowStripe" dxfId="59"/>
-      <tableStyleElement type="secondRowStripe" dxfId="58"/>
+      <tableStyleElement type="headerRow" dxfId="59"/>
+      <tableStyleElement type="firstRowStripe" dxfId="58"/>
+      <tableStyleElement type="secondRowStripe" dxfId="57"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 5" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
-      <tableStyleElement type="headerRow" dxfId="57"/>
-      <tableStyleElement type="firstRowStripe" dxfId="56"/>
-      <tableStyleElement type="secondRowStripe" dxfId="55"/>
+      <tableStyleElement type="headerRow" dxfId="56"/>
+      <tableStyleElement type="firstRowStripe" dxfId="55"/>
+      <tableStyleElement type="secondRowStripe" dxfId="54"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 6" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
-      <tableStyleElement type="headerRow" dxfId="54"/>
-      <tableStyleElement type="firstRowStripe" dxfId="53"/>
-      <tableStyleElement type="secondRowStripe" dxfId="52"/>
+      <tableStyleElement type="headerRow" dxfId="53"/>
+      <tableStyleElement type="firstRowStripe" dxfId="52"/>
+      <tableStyleElement type="secondRowStripe" dxfId="51"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 7" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
-      <tableStyleElement type="headerRow" dxfId="51"/>
-      <tableStyleElement type="firstRowStripe" dxfId="50"/>
-      <tableStyleElement type="secondRowStripe" dxfId="49"/>
+      <tableStyleElement type="headerRow" dxfId="50"/>
+      <tableStyleElement type="firstRowStripe" dxfId="49"/>
+      <tableStyleElement type="secondRowStripe" dxfId="48"/>
     </tableStyle>
     <tableStyle name="Worksheet-style 8" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF07000000}">
-      <tableStyleElement type="headerRow" dxfId="48"/>
-      <tableStyleElement type="firstRowStripe" dxfId="47"/>
-      <tableStyleElement type="secondRowStripe" dxfId="46"/>
+      <tableStyleElement type="headerRow" dxfId="47"/>
+      <tableStyleElement type="firstRowStripe" dxfId="46"/>
+      <tableStyleElement type="secondRowStripe" dxfId="45"/>
     </tableStyle>
     <tableStyle name="Cloud.gov Tiers-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF08000000}">
-      <tableStyleElement type="headerRow" dxfId="45"/>
-      <tableStyleElement type="firstRowStripe" dxfId="44"/>
-      <tableStyleElement type="secondRowStripe" dxfId="43"/>
+      <tableStyleElement type="headerRow" dxfId="44"/>
+      <tableStyleElement type="firstRowStripe" dxfId="43"/>
+      <tableStyleElement type="secondRowStripe" dxfId="42"/>
     </tableStyle>
     <tableStyle name="Cloud.gov Tiers-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF09000000}">
-      <tableStyleElement type="headerRow" dxfId="42"/>
-      <tableStyleElement type="firstRowStripe" dxfId="41"/>
-      <tableStyleElement type="secondRowStripe" dxfId="40"/>
+      <tableStyleElement type="headerRow" dxfId="41"/>
+      <tableStyleElement type="firstRowStripe" dxfId="40"/>
+      <tableStyleElement type="secondRowStripe" dxfId="39"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -3052,20 +3078,20 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A4:F5">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Credits" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tier Name" dataDxfId="38">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Credits" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tier Name" dataDxfId="37">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.Tier, VLOOKUP(MIN(IF('Cloud.gov Tiers'!$B$11:$B$28&gt;=A5, 'Cloud.gov Tiers'!$B$11:$B$28)), 'Cloud.gov Tiers'!$B$11:$E$28, 4, FALSE), VLOOKUP(_xlpm.Tier, 'Cloud.gov Tiers'!$E$10:$F$28, 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Credits Remaining_x000a_in Tier" dataDxfId="37">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Credits Remaining_x000a_in Tier" dataDxfId="36">
       <calculatedColumnFormula>VLOOKUP(Table_1[[#This Row],[Tier Name]], 'Cloud.gov Tiers'!A11:B27, 2,FALSE)-Table_1[[#This Row],[Credits]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Yearly_x000a_Platform Total" dataDxfId="36">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Yearly_x000a_Platform Total" dataDxfId="35">
       <calculatedColumnFormula>IF(B5="Custom", ROUNDUP(A5/1000,0)*'Cloud.gov Tiers'!$H$28, VLOOKUP(B5, 'Cloud.gov Tiers'!$F$11:$H$27, 3, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Support Total" dataDxfId="35">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Support Total" dataDxfId="34">
       <calculatedColumnFormula>C15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name=" YearlyTotal Cost" dataDxfId="34">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name=" YearlyTotal Cost" dataDxfId="33">
       <calculatedColumnFormula>D5+E5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3074,6 +3100,16 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table_9" displayName="Table_9" ref="A2:B6">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Variable"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="Cloud.gov Tiers-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table_10" displayName="Table_10" ref="A10:H28">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Tier"/>
@@ -3093,7 +3129,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A9:C10">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Resource"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Quantity" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Quantity" dataDxfId="32"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Credits"/>
   </tableColumns>
   <tableStyleInfo name="Worksheet-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -3103,13 +3139,13 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="E9:K10">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Offering" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Description" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Dimension" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="GB per credit" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Quantity (GB)" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Credits" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Offering" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Description" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Dimension" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="GB per credit" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Quantity (GB)" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Credits" dataDxfId="25">
       <calculatedColumnFormula>ROUNDUP(Table_3[[#This Row],[Quantity (GB)]]/Table_3[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3123,12 +3159,12 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Offering"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Units"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Dimension" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{CDA60C5E-AE6A-324F-8F61-A71F1A0A8966}" name="GB per credit" dataDxfId="29">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Dimension" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{CDA60C5E-AE6A-324F-8F61-A71F1A0A8966}" name="GB per credit" dataDxfId="23">
       <calculatedColumnFormula>'AWS Service Prices'!K5*'AWS Service Prices'!M5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Quantity (GB)" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Credits" dataDxfId="30">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Quantity (GB)" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Credits" dataDxfId="21">
       <calculatedColumnFormula>ROUNDUP(Table_4[[#This Row],[Quantity (GB)]]/Table_4[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3140,7 +3176,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="A14:C15">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Rate/Hour"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Hours" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Hours" dataDxfId="20"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Total"/>
   </tableColumns>
   <tableStyleInfo name="Worksheet-style 5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -3150,15 +3186,15 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_6" displayName="Table_6" ref="M14:S15" dataDxfId="19">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Offering" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Description" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Units" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Dimension" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{807927EE-801B-8148-9BA1-5FE9186170F2}" name="GB per credit" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Offering" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Description" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Units" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Dimension" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{807927EE-801B-8148-9BA1-5FE9186170F2}" name="GB per credit" dataDxfId="14">
       <calculatedColumnFormula>'AWS Service Prices'!K4*'AWS Service Prices'!M4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Quantity (GB)" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Credits" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Quantity (GB)" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Credits" dataDxfId="12">
       <calculatedColumnFormula>ROUNDUP(Table_6[[#This Row],[Quantity (GB)]]/Table_6[[#This Row],[GB per credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3183,11 +3219,11 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Units"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Dimension"/>
-    <tableColumn id="3" xr3:uid="{A30E673E-5221-9442-BA33-5D5CC8E273B5}" name="Units/Credit" dataDxfId="31">
+    <tableColumn id="3" xr3:uid="{A30E673E-5221-9442-BA33-5D5CC8E273B5}" name="Units/Credit" dataDxfId="11">
       <calculatedColumnFormula>'AWS Service Prices'!K6*'AWS Service Prices'!M6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Quantity"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Credits" dataDxfId="18">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Credits" dataDxfId="10">
       <calculatedColumnFormula>ROUNDUP(Table_8[[#This Row],[Quantity]]/Table_8[[#This Row],[Units/Credit]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3196,12 +3232,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table_9" displayName="Table_9" ref="A2:B6">
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Variable"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Value"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}" name="Table12" displayName="Table12" ref="A39:C49" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="9">
+  <autoFilter ref="A39:C49" xr:uid="{834417E1-38BD-134B-B77F-84AFCA28E8D3}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6F594386-932F-3745-B570-1D36152A4BED}" name="Version" dataDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{98BA1600-A7B8-2742-AF88-1C465CCF83D5}" name="Date"/>
+    <tableColumn id="3" xr3:uid="{A3A06425-E98A-E042-A27B-C92165F08BCF}" name="Notes"/>
   </tableColumns>
-  <tableStyleInfo name="Cloud.gov Tiers-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="Cloud.gov Tiers-style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3410,14 +3448,14 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S42" sqref="S42"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="30.83203125" customWidth="1"/>
@@ -3440,14 +3478,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="98.25" customHeight="1" x14ac:dyDescent="1.05">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3703,7 +3741,7 @@
       <c r="J14" s="20">
         <v>2</v>
       </c>
-      <c r="K14" s="92">
+      <c r="K14" s="90">
         <f>I14*J14</f>
         <v>2</v>
       </c>
@@ -3758,7 +3796,7 @@
       <c r="J15" s="26">
         <v>0</v>
       </c>
-      <c r="K15" s="92">
+      <c r="K15" s="90">
         <f t="shared" ref="K15:K43" si="0">I15*J15</f>
         <v>0</v>
       </c>
@@ -3805,7 +3843,7 @@
       <c r="J16" s="26">
         <v>0</v>
       </c>
-      <c r="K16" s="92">
+      <c r="K16" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3832,7 +3870,7 @@
       <c r="J17" s="26">
         <v>1</v>
       </c>
-      <c r="K17" s="92">
+      <c r="K17" s="90">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -3866,7 +3904,7 @@
       <c r="J18" s="26">
         <v>0</v>
       </c>
-      <c r="K18" s="92">
+      <c r="K18" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3918,7 +3956,7 @@
       <c r="J19" s="26">
         <v>0</v>
       </c>
-      <c r="K19" s="92">
+      <c r="K19" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3972,7 +4010,7 @@
       <c r="J20" s="26">
         <v>0</v>
       </c>
-      <c r="K20" s="92">
+      <c r="K20" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4025,7 +4063,7 @@
       <c r="J21" s="26">
         <v>0</v>
       </c>
-      <c r="K21" s="92">
+      <c r="K21" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4078,7 +4116,7 @@
       <c r="J22" s="35">
         <v>0</v>
       </c>
-      <c r="K22" s="92">
+      <c r="K22" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4131,7 +4169,7 @@
       <c r="J23" s="26">
         <v>0</v>
       </c>
-      <c r="K23" s="92">
+      <c r="K23" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4177,7 +4215,7 @@
       <c r="J24" s="26">
         <v>0</v>
       </c>
-      <c r="K24" s="92">
+      <c r="K24" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4223,7 +4261,7 @@
       <c r="J25" s="26">
         <v>0</v>
       </c>
-      <c r="K25" s="92">
+      <c r="K25" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4272,7 +4310,7 @@
       <c r="J26" s="26">
         <v>0</v>
       </c>
-      <c r="K26" s="92">
+      <c r="K26" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4324,7 +4362,7 @@
       <c r="J27" s="26">
         <v>0</v>
       </c>
-      <c r="K27" s="92">
+      <c r="K27" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4377,7 +4415,7 @@
       <c r="J28" s="26">
         <v>0</v>
       </c>
-      <c r="K28" s="92">
+      <c r="K28" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4429,7 +4467,7 @@
       <c r="J29" s="26">
         <v>0</v>
       </c>
-      <c r="K29" s="92">
+      <c r="K29" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4451,11 +4489,11 @@
       <c r="R29" s="41">
         <v>0</v>
       </c>
-      <c r="S29" s="93">
+      <c r="S29" s="91">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T29" s="94"/>
+      <c r="T29" s="92"/>
     </row>
     <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="18" t="str">
@@ -4482,7 +4520,7 @@
       <c r="J30" s="43">
         <v>0</v>
       </c>
-      <c r="K30" s="92">
+      <c r="K30" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4514,7 +4552,7 @@
       <c r="J31" s="26">
         <v>0</v>
       </c>
-      <c r="K31" s="92">
+      <c r="K31" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4552,7 +4590,7 @@
       <c r="J32" s="26">
         <v>0</v>
       </c>
-      <c r="K32" s="92">
+      <c r="K32" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4603,7 +4641,7 @@
       <c r="J33" s="26">
         <v>0</v>
       </c>
-      <c r="K33" s="92">
+      <c r="K33" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4620,7 +4658,7 @@
       <c r="P33" s="48">
         <v>1</v>
       </c>
-      <c r="Q33" s="90">
+      <c r="Q33" s="88">
         <v>1</v>
       </c>
       <c r="R33" s="50">
@@ -4656,7 +4694,7 @@
       <c r="J34" s="26">
         <v>0</v>
       </c>
-      <c r="K34" s="92">
+      <c r="K34" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4672,7 +4710,7 @@
       <c r="P34" s="25">
         <v>3</v>
       </c>
-      <c r="Q34" s="90">
+      <c r="Q34" s="88">
         <v>2</v>
       </c>
       <c r="R34" s="38">
@@ -4708,7 +4746,7 @@
       <c r="J35" s="35">
         <v>0</v>
       </c>
-      <c r="K35" s="92">
+      <c r="K35" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4724,7 +4762,7 @@
       <c r="P35" s="48">
         <v>5</v>
       </c>
-      <c r="Q35" s="90">
+      <c r="Q35" s="88">
         <v>4</v>
       </c>
       <c r="R35" s="38">
@@ -4758,7 +4796,7 @@
       <c r="J36" s="26">
         <v>0</v>
       </c>
-      <c r="K36" s="92">
+      <c r="K36" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4774,7 +4812,7 @@
       <c r="P36" s="25">
         <v>3</v>
       </c>
-      <c r="Q36" s="90">
+      <c r="Q36" s="88">
         <v>5</v>
       </c>
       <c r="R36" s="38">
@@ -4804,7 +4842,7 @@
       <c r="J37" s="26">
         <v>0</v>
       </c>
-      <c r="K37" s="92">
+      <c r="K37" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4820,13 +4858,13 @@
       <c r="P37" s="40">
         <v>5</v>
       </c>
-      <c r="Q37" s="91">
+      <c r="Q37" s="89">
         <v>8</v>
       </c>
       <c r="R37" s="45">
         <v>0</v>
       </c>
-      <c r="S37" s="93">
+      <c r="S37" s="91">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4850,12 +4888,21 @@
       <c r="J38" s="26">
         <v>0</v>
       </c>
-      <c r="K38" s="92">
+      <c r="K38" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="104" t="s">
+        <v>183</v>
+      </c>
+      <c r="B39" s="105" t="s">
+        <v>184</v>
+      </c>
+      <c r="C39" s="106" t="s">
+        <v>185</v>
+      </c>
       <c r="E39" s="24" t="str">
         <v>AWS RDS</v>
       </c>
@@ -4874,7 +4921,7 @@
       <c r="J39" s="26">
         <v>0</v>
       </c>
-      <c r="K39" s="92">
+      <c r="K39" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4883,6 +4930,15 @@
       </c>
     </row>
     <row r="40" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="107">
+        <v>1</v>
+      </c>
+      <c r="B40" s="103">
+        <v>45748</v>
+      </c>
+      <c r="C40" s="102" t="s">
+        <v>189</v>
+      </c>
       <c r="E40" s="18" t="str">
         <v>AWS RDS</v>
       </c>
@@ -4901,7 +4957,7 @@
       <c r="J40" s="26">
         <v>0</v>
       </c>
-      <c r="K40" s="92">
+      <c r="K40" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4923,11 +4979,20 @@
       <c r="R40" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="S40" s="97" t="s">
+      <c r="S40" s="95" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="107">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B41" s="103">
+        <v>45749</v>
+      </c>
+      <c r="C41" s="102" t="s">
+        <v>186</v>
+      </c>
       <c r="E41" s="24" t="str">
         <v>AWS RDS</v>
       </c>
@@ -4946,7 +5011,7 @@
       <c r="J41" s="26">
         <v>0</v>
       </c>
-      <c r="K41" s="92">
+      <c r="K41" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4962,19 +5027,23 @@
       <c r="P41" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="Q41" s="90">
+      <c r="Q41" s="88">
         <f>'AWS Service Prices'!K6*'AWS Service Prices'!M6</f>
         <v>150000</v>
       </c>
-      <c r="R41" s="95">
+      <c r="R41" s="93">
         <v>10000</v>
       </c>
-      <c r="S41" s="99">
+      <c r="S41" s="97">
         <f>ROUNDUP(Table_8[[#This Row],[Quantity]]/Table_8[[#This Row],[Units/Credit]],0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="107"/>
+      <c r="C42" s="102" t="s">
+        <v>187</v>
+      </c>
       <c r="E42" s="18" t="str">
         <v>AWS RDS</v>
       </c>
@@ -4993,7 +5062,7 @@
       <c r="J42" s="26">
         <v>0</v>
       </c>
-      <c r="K42" s="92">
+      <c r="K42" s="90">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5009,19 +5078,23 @@
       <c r="P42" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="Q42" s="90">
+      <c r="Q42" s="88">
         <f>'AWS Service Prices'!K7*'AWS Service Prices'!M7</f>
         <v>120</v>
       </c>
-      <c r="R42" s="96">
+      <c r="R42" s="94">
         <v>2</v>
       </c>
-      <c r="S42" s="98">
+      <c r="S42" s="96">
         <f>ROUNDUP(Table_8[[#This Row],[Quantity]]/Table_8[[#This Row],[Units/Credit]],0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="107"/>
+      <c r="C43" s="102" t="s">
+        <v>188</v>
+      </c>
       <c r="E43" s="54" t="str">
         <v>AWS RDS</v>
       </c>
@@ -5040,73 +5113,80 @@
       <c r="J43" s="56">
         <v>0</v>
       </c>
-      <c r="K43" s="101">
+      <c r="K43" s="99">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q43" s="100"/>
+      <c r="Q43" s="98"/>
     </row>
     <row r="44" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="107"/>
       <c r="J44" s="4"/>
     </row>
     <row r="45" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="107"/>
       <c r="J45" s="4"/>
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="107"/>
       <c r="J46" s="4"/>
     </row>
     <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="107"/>
       <c r="J47" s="4"/>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="107"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="107"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="107"/>
       <c r="J50" s="4"/>
     </row>
-    <row r="51" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J52" s="4"/>
     </row>
-    <row r="53" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J54" s="4"/>
     </row>
-    <row r="55" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J58" s="4"/>
     </row>
-    <row r="59" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J59" s="4"/>
     </row>
-    <row r="60" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J60" s="4"/>
     </row>
-    <row r="61" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J61" s="4"/>
     </row>
-    <row r="62" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J62" s="4"/>
     </row>
-    <row r="63" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J63" s="4"/>
     </row>
-    <row r="64" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J64" s="4"/>
     </row>
     <row r="65" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6078,43 +6158,43 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="B10 J14:J43 B15">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R10">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R15">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R19:R29">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R33:R37">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R41:R42">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R19:R29">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R33:R37">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R15">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <tableParts count="8">
+  <tableParts count="9">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -6123,6 +6203,7 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7789,7 +7870,7 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="K3" sqref="K3:M3"/>
     </sheetView>
   </sheetViews>

</xml_diff>